<commit_message>
Pequena Alteração no Doc dos Requisitos
</commit_message>
<xml_diff>
--- a/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
+++ b/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\CANDIDATURAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BA9C35-381A-41A4-B34A-BD280036B711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B87BEE-4419-4213-A151-1F913EBA744E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
   </bookViews>
   <sheets>
-    <sheet name="DADOS SIMPLES" sheetId="4" r:id="rId1"/>
-    <sheet name="DADOS FORMATADOS" sheetId="2" r:id="rId2"/>
-    <sheet name="DADOS CLASSIFICADOS" sheetId="3" r:id="rId3"/>
-    <sheet name="DADOS ELIANA" sheetId="5" r:id="rId4"/>
-    <sheet name="RESUMO ELIANA" sheetId="6" r:id="rId5"/>
+    <sheet name="REQUISITOS DO PROJETO" sheetId="9" r:id="rId1"/>
+    <sheet name="DADOS SIMPLES" sheetId="4" r:id="rId2"/>
+    <sheet name="DADOS FORMATADOS" sheetId="2" r:id="rId3"/>
+    <sheet name="DADOS CLASSIFICADOS" sheetId="3" r:id="rId4"/>
+    <sheet name="DADOS ELIANA" sheetId="5" r:id="rId5"/>
+    <sheet name="RESUMO ELIANA" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'DADOS CLASSIFICADOS'!$A$1:$I$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'DADOS CLASSIFICADOS'!$A$1:$I$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="156">
   <si>
     <t>TIPO</t>
   </si>
@@ -180,24 +181,9 @@
     <t>Seus vendedores afiliados</t>
   </si>
   <si>
-    <t>Soma</t>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Soma Acumulada</t>
-  </si>
-  <si>
-    <t>Contagem</t>
-  </si>
-  <si>
     <t>Comissão Paga aos vendedores</t>
   </si>
   <si>
-    <t>Valor recebido pelo afiliado</t>
-  </si>
-  <si>
     <t>Eliana vendeu</t>
   </si>
   <si>
@@ -214,6 +200,587 @@
   </si>
   <si>
     <t>Saldo Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>| Tipo | Descrição         | Natureza | Sinal |</t>
+  </si>
+  <si>
+    <t>| ---- | ----------------- | -------- | ----- |</t>
+  </si>
+  <si>
+    <t>| 1    | Venda produtor    | Entrada  | +     |</t>
+  </si>
+  <si>
+    <t>| 2    | Venda afiliado    | Entrada  | +     |</t>
+  </si>
+  <si>
+    <t>| 3    | Comissão paga     | Saída    | -     |</t>
+  </si>
+  <si>
+    <t>| 4    | Comissão recebida | Entrada  | +     |</t>
+  </si>
+  <si>
+    <t>podendo ser do produtor ou afiliado.</t>
+  </si>
+  <si>
+    <t># Desafio de programação</t>
+  </si>
+  <si>
+    <t>O objetivo desse teste é avaliar as suas habilidades em programação.</t>
+  </si>
+  <si>
+    <t>## Descrição do projeto</t>
+  </si>
+  <si>
+    <t>Surgiu uma nova demanda urgente e precisamos de uma área exclusiva para fazer o</t>
+  </si>
+  <si>
+    <t>upload de um arquivo das transações feitas na venda de produtos por nossos</t>
+  </si>
+  <si>
+    <t>clientes.</t>
+  </si>
+  <si>
+    <t>produtos, desde que seja paga uma comissão por venda.</t>
+  </si>
+  <si>
+    <t>banco de dados relacional.</t>
+  </si>
+  <si>
+    <t>## Configurando Seu Ambiente</t>
+  </si>
+  <si>
+    <t>1. No diretório onde você descompactou o arquivo do desafio crie um repo git e</t>
+  </si>
+  <si>
+    <t>   uma branch:</t>
+  </si>
+  <si>
+    <t>   git init --initial-branch=main</t>
+  </si>
+  <si>
+    <t>   git checkout -b desafio</t>
+  </si>
+  <si>
+    <t>2. Desenvolva o desafio fazendo commits no repositório.</t>
+  </si>
+  <si>
+    <t>## Requisitos Funcionais</t>
+  </si>
+  <si>
+    <t>Sua aplicação deve:</t>
+  </si>
+  <si>
+    <t>1. Ter uma tela (via formulário) para fazer o upload do arquivo</t>
+  </si>
+  <si>
+    <t>2. Fazer o parsing do arquivo recebido, normalizar os dados e armazená-los em um</t>
+  </si>
+  <si>
+    <t>   banco de dados relacional, seguindo as definições de interpretação do arquivo</t>
+  </si>
+  <si>
+    <t>3. Exibir a lista de todas as transações de produtos importadas</t>
+  </si>
+  <si>
+    <t>4. Exibir o saldo final do produtor</t>
+  </si>
+  <si>
+    <t>5. Exibir o saldo final de um afiliado</t>
+  </si>
+  <si>
+    <t>6. Fazer tratamento de erros no backend, e reportar mensagens de erro amigáveis</t>
+  </si>
+  <si>
+    <t>   no frontend.</t>
+  </si>
+  <si>
+    <t>## Requisitos Não Funcionais</t>
+  </si>
+  <si>
+    <t>1. Escreva um README descrevendo o projeto e como fazer o setup.</t>
+  </si>
+  <si>
+    <t>1. A aplicação deve ser simples de configurar e rodar, compatível com ambiente</t>
+  </si>
+  <si>
+    <t>1. Utilize docker para os diferentes serviços que compõe a aplicação para que</t>
+  </si>
+  <si>
+    <t>   funcione facilmente fora do seu ambiente pessoal.</t>
+  </si>
+  <si>
+    <t>1. Use commits pequenos no Git e escreva uma boa descrição para cada um.</t>
+  </si>
+  <si>
+    <t>1. Faça o código mais legível e limpo possível.</t>
+  </si>
+  <si>
+    <t>   português se preferir.</t>
+  </si>
+  <si>
+    <t>1. Grave um vídeo de poucos minutos (até 5) mostrando sua solução em</t>
+  </si>
+  <si>
+    <t>   funcionamento. Mesmo usando Docker já tivemos problemas.</t>
+  </si>
+  <si>
+    <t>   Isso vai nos dar mais velocidade e agilidade para corrigir. Se não puder</t>
+  </si>
+  <si>
+    <t>   gravar um vídeo, adicione imagens de todas as telas (mas o vídeo é</t>
+  </si>
+  <si>
+    <t>   preferível). Ferramenta para gravar tela:</t>
+  </si>
+  <si>
+    <t>   - Windows, Mac, Linux: OBS Studio</t>
+  </si>
+  <si>
+    <t>   - Mac: gravador nativo (basta apertar cmd+shift+5)</t>
+  </si>
+  <si>
+    <t>   Se o vídeo tiver tamanho final menor que 25mb, o que é improvável, pode</t>
+  </si>
+  <si>
+    <t>   enviar por email mesmo. Do contrário, pode ser tanto por um link do Google</t>
+  </si>
+  <si>
+    <t>   Drive ou do YouTube (não listado). Ambos gratuitos.</t>
+  </si>
+  <si>
+    <t>## Requisitos Bônus</t>
+  </si>
+  <si>
+    <t>Sua aplicação não precisa, mas ficaremos impressionados se ela:</t>
+  </si>
+  <si>
+    <t>1. Tiver documentação das APIs do backend.</t>
+  </si>
+  <si>
+    <t>2. Utilizar docker-compose para orquestar os serviços num todo.</t>
+  </si>
+  <si>
+    <t>3. Ter testes de integração ou end-to-end.</t>
+  </si>
+  <si>
+    <t>4. Tiver toda a documentação escrita em inglês fácil de entender.</t>
+  </si>
+  <si>
+    <t>5. Lidar com autenticação e/ou autorização. OK</t>
+  </si>
+  <si>
+    <t>## Formato do arquivo de entrada</t>
+  </si>
+  <si>
+    <t>| Campo    | Início | Fim | Tamanho | Descrição                      |</t>
+  </si>
+  <si>
+    <t>| -------- | ------ | --- | ------- | ------------------------------ |</t>
+  </si>
+  <si>
+    <t>| Tipo     | 1      | 1   | 1       | Tipo da transação              |</t>
+  </si>
+  <si>
+    <t>| Data     | 2      | 26  | 25      | Data - ISO Date + GMT          |</t>
+  </si>
+  <si>
+    <t>| Produto  | 27     | 56  | 30      | Descrição do produto           |</t>
+  </si>
+  <si>
+    <t>| Valor    | 57     | 66  | 10      | Valor da transação em centavos |</t>
+  </si>
+  <si>
+    <t>| Vendedor | 67     | 86  | 20      | Nome do vendedor               |</t>
+  </si>
+  <si>
+    <t>### Tipos de transação</t>
+  </si>
+  <si>
+    <t>Esses são os valores possíveis para o campo Tipo:</t>
+  </si>
+  <si>
+    <t>## Avaliação</t>
+  </si>
+  <si>
+    <t>Seu projeto será avaliado de acordo com os seguintes critérios:</t>
+  </si>
+  <si>
+    <t>1. Documentação do setup do ambiente e execução que rode a aplicação com</t>
+  </si>
+  <si>
+    <t>   sucesso.</t>
+  </si>
+  <si>
+    <t>3. Boa estruturação do componentes e layout de código, mas sem over engineering.</t>
+  </si>
+  <si>
+    <t>4. Legibilidade do código.</t>
+  </si>
+  <si>
+    <t>5. Boa cobertura de testes.</t>
+  </si>
+  <si>
+    <t>6. Claridade e extensão da documentação.</t>
+  </si>
+  <si>
+    <t>## Entregando a Resposta do Desafio</t>
+  </si>
+  <si>
+    <t>   git bundle create nome-sobrenome.bundle HEAD desafio</t>
+  </si>
+  <si>
+    <t>2. Envie o arquivo do bundle para nós via email, para a mesma pessoa que te</t>
+  </si>
+  <si>
+    <t>   enviou o desafio.</t>
+  </si>
+  <si>
+    <t>#### Verificar o bundle</t>
+  </si>
+  <si>
+    <t>Para verificar o arquivo antes de enviar utilize o seguinte comando:</t>
+  </si>
+  <si>
+    <t>```</t>
+  </si>
+  <si>
+    <t>git clone nome-sobrenome.bundle hubla-take-home</t>
+  </si>
+  <si>
+    <t>## Boa Sorte!!!</t>
+  </si>
+  <si>
+    <r>
+      <t>Você deve utilizar o arquivo [sales.txt](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sales.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) para fazer o teste da</t>
+    </r>
+  </si>
+  <si>
+    <t>   ```bash</t>
+  </si>
+  <si>
+    <t>   ```</t>
+  </si>
+  <si>
+    <r>
+      <t>2. Cumprimento dos [requisitos funcionais](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#Requisitos-Funcionais</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) e</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>   [não funcionais](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#Requisitos-Nao-Funcionais</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7. Cumprimento de algum [requisito bônus](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#Requisitos-Bonus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Crie um [git bundle](</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>https://git-scm.com/docs/git-bundle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) com o seu trabalho:</t>
+    </r>
+  </si>
+  <si>
+    <t>A cópia do seu trabalho vai estar em `hubla-take-home`.</t>
+  </si>
+  <si>
+    <t>Saida</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nossa plataforma trabalha no modelo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>criador-afiliado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, sendo assim </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>um criador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>pode vender seus produtos e ter 1 ou mais afiliados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> também vendendo esses</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Uma transação financeira é um contrato de compra e venda.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> No contexto do</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">enunciado, vamos considerar que </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cada transação resulta na mudança do saldo,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sua tarefa é construir uma interface web que possibilite o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>upload de um arquivo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">de transações de produtos vendidos, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>normalizar os dados e armazená-los</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> em um</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">aplicação. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>O formato esá descrito na seção "Formato do arquivo de entrada".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   Unix. Você deve utilizar </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>apenas bibliotecas gratuitas ou livres.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>qualquer banco de dados relacional.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Escreva </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>unit tests tanto no backend quanto do frontend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Escreva o código (nomes e comentários) em inglês. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>A documentação pode ser em</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -221,9 +788,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="179" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,8 +878,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="19"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF7030A0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +973,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF13141F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,7 +1118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,13 +1161,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -544,9 +1170,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -559,9 +1182,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -574,56 +1194,37 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="179" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -633,36 +1234,76 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="9" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,11 +1617,660 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EBEA93-B706-48A3-924F-8B7166C6FDE2}">
+  <dimension ref="A1:A140"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="112.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="66"/>
+    </row>
+    <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="66"/>
+    </row>
+    <row r="5" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="66"/>
+    </row>
+    <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="66"/>
+    </row>
+    <row r="11" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="67" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="66"/>
+    </row>
+    <row r="15" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="67" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="67" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="66"/>
+    </row>
+    <row r="19" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="67" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="67" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="66"/>
+    </row>
+    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="67" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="67" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="66"/>
+    </row>
+    <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="66"/>
+    </row>
+    <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="67" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="67" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="66"/>
+    </row>
+    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="66"/>
+    </row>
+    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="67" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="66"/>
+    </row>
+    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="67" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="67" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="67" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="67" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="66"/>
+    </row>
+    <row r="49" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="65" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="66"/>
+    </row>
+    <row r="51" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="67" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="67" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="75" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="67" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="67" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="66"/>
+    </row>
+    <row r="65" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="67" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="67" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="66"/>
+    </row>
+    <row r="69" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="66"/>
+    </row>
+    <row r="72" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="66"/>
+    </row>
+    <row r="76" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="66"/>
+    </row>
+    <row r="78" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="67" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="66"/>
+    </row>
+    <row r="80" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="76" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="65" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="67" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="76" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="74" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="66"/>
+    </row>
+    <row r="86" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="66"/>
+    </row>
+    <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="67" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="67" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="67" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="67" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="66"/>
+    </row>
+    <row r="96" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="66"/>
+    </row>
+    <row r="98" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="66"/>
+    </row>
+    <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="67" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="67" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="66"/>
+    </row>
+    <row r="107" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="65" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="66"/>
+    </row>
+    <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="66"/>
+    </row>
+    <row r="111" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="76" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="67" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="67" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="76" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="67" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="66"/>
+    </row>
+    <row r="121" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="66"/>
+    </row>
+    <row r="123" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="67" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="67" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A125" s="67" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="67" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="67" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="67" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="66"/>
+    </row>
+    <row r="130" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="66"/>
+    </row>
+    <row r="132" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="66"/>
+    </row>
+    <row r="134" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="66"/>
+    </row>
+    <row r="138" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="66"/>
+    </row>
+    <row r="140" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A140" s="65" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EDDACD-BA6F-4CED-8353-4C1EA0202EBE}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G4" sqref="G4:Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +2282,7 @@
     <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +2299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1025,8 +2315,12 @@
       <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(A2:E2)</f>
+        <v>12022-01-15T19: 20: 30-03: 00CURSO DE BEM-ESTAR      0000012750JOSE CARLOS</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1043,7 +2337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1059,8 +2353,21 @@
       <c r="E4" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G4" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+    </row>
+    <row r="5" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1076,8 +2383,21 @@
       <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G5" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+    </row>
+    <row r="6" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -1093,8 +2413,21 @@
       <c r="E6" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G6" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+    </row>
+    <row r="7" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1110,8 +2443,21 @@
       <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G7" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+    </row>
+    <row r="8" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -1127,8 +2473,21 @@
       <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G8" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+    </row>
+    <row r="9" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>2</v>
       </c>
@@ -1144,8 +2503,21 @@
       <c r="E9" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G9" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="63"/>
+    </row>
+    <row r="10" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -1161,8 +2533,19 @@
       <c r="E10" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="63"/>
+    </row>
+    <row r="11" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>2</v>
       </c>
@@ -1179,7 +2562,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>4</v>
       </c>
@@ -1195,8 +2578,9 @@
       <c r="E12" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G12" s="64"/>
+    </row>
+    <row r="13" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -1212,8 +2596,9 @@
       <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G13" s="64"/>
+    </row>
+    <row r="14" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>4</v>
       </c>
@@ -1229,8 +2614,9 @@
       <c r="E14" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="G14" s="64"/>
+    </row>
+    <row r="15" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>3</v>
       </c>
@@ -1247,7 +2633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>3</v>
       </c>
@@ -1354,12 +2740,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7EA72D-CE26-4056-ACD9-087E17A333AD}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +2756,7 @@
     <col min="4" max="4" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1393,7 +2779,7 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1419,7 +2805,7 @@
       <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="12">
         <v>12750</v>
       </c>
       <c r="H2" s="13" t="s">
@@ -1445,7 +2831,7 @@
       <c r="F3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="12">
         <v>50000</v>
       </c>
       <c r="H3" s="13" t="s">
@@ -1453,80 +2839,80 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="18">
         <v>12750</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="24">
+      <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="22">
         <v>4500</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="29">
+      <c r="A6" s="24">
         <v>3</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="26">
         <v>4500</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="27" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1549,7 +2935,7 @@
       <c r="F7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="12">
         <v>50000</v>
       </c>
       <c r="H7" s="13" t="s">
@@ -1575,7 +2961,7 @@
       <c r="F8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="12">
         <v>155000</v>
       </c>
       <c r="H8" s="13" t="s">
@@ -1583,236 +2969,236 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="19">
+      <c r="A9" s="16">
         <v>2</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="22">
+      <c r="F9" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="18">
         <v>155000</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="19">
+      <c r="A10" s="16">
         <v>2</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="22">
+      <c r="F10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="18">
         <v>155000</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="19">
+      <c r="A11" s="16">
         <v>2</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="22">
+      <c r="F11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="18">
         <v>155000</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="24">
+      <c r="A12" s="20">
         <v>4</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="27">
+      <c r="F12" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="22">
         <v>50000</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="24">
+      <c r="A13" s="20">
         <v>4</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="27">
+      <c r="F13" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="22">
         <v>50000</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="H13" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="24">
+      <c r="A14" s="20">
         <v>4</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="27">
+      <c r="F14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="22">
         <v>50000</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="29">
+      <c r="A15" s="24">
         <v>3</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="32">
+      <c r="F15" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="26">
         <v>50000</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H15" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="29">
+      <c r="A16" s="24">
         <v>3</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="32">
+      <c r="F16" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="26">
         <v>50000</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="29">
+      <c r="A17" s="24">
         <v>3</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="32">
+      <c r="F17" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="26">
         <v>50000</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="H17" s="27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1835,7 +3221,7 @@
       <c r="F18" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="12">
         <v>50000</v>
       </c>
       <c r="H18" s="13" t="s">
@@ -1861,7 +3247,7 @@
       <c r="F19" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="12">
         <v>12750</v>
       </c>
       <c r="H19" s="13" t="s">
@@ -1887,7 +3273,7 @@
       <c r="F20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="12">
         <v>155000</v>
       </c>
       <c r="H20" s="13" t="s">
@@ -1913,7 +3299,7 @@
       <c r="F21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="12">
         <v>155000</v>
       </c>
       <c r="H21" s="13" t="s">
@@ -1925,12 +3311,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +3353,7 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="14" t="s">
@@ -1978,365 +3364,365 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="19">
-        <v>2</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="21" t="s">
+      <c r="A2" s="24">
+        <v>3</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="22">
-        <v>155000</v>
-      </c>
-      <c r="H2" s="34">
-        <f>G2/100</f>
-        <v>1550</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
+      <c r="F2" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="26">
+        <v>50000</v>
+      </c>
+      <c r="H2" s="45">
+        <f t="shared" ref="H2:H21" si="0">G2/100</f>
+        <v>500</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="29"/>
+      <c r="K2" s="30"/>
     </row>
     <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="26">
+        <v>50000</v>
+      </c>
+      <c r="H3" s="45">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="I3" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="24">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="26">
+        <v>50000</v>
+      </c>
+      <c r="H4" s="45">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="24">
+        <v>3</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="26">
+        <v>4500</v>
+      </c>
+      <c r="H5" s="45">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="20">
+        <v>4</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D6" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="27">
+      <c r="F6" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="22">
         <v>50000</v>
       </c>
-      <c r="H3" s="40">
-        <f t="shared" ref="H3:H21" si="0">G3/100</f>
+      <c r="H6" s="32">
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I6" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="20">
+        <v>4</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="22">
+        <v>50000</v>
+      </c>
+      <c r="H7" s="32">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="20">
+        <v>4</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="22">
+        <v>50000</v>
+      </c>
+      <c r="H8" s="32">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="20">
+        <v>4</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="22">
+        <v>4500</v>
+      </c>
+      <c r="H9" s="32">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B10" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D10" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="22">
+      <c r="E10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="18">
         <v>155000</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H10" s="28">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="24">
-        <v>4</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="25" t="s">
+      <c r="I10" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="16">
+        <v>2</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E11" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="27">
-        <v>50000</v>
-      </c>
-      <c r="H5" s="40">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I5" s="28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
-        <v>2</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="22">
+      <c r="F11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="18">
         <v>155000</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H11" s="28">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="24">
-        <v>4</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="25" t="s">
+      <c r="I11" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="16">
+        <v>2</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="27">
-        <v>50000</v>
-      </c>
-      <c r="H7" s="40">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I7" s="28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="17">
+      <c r="F12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="18">
         <v>155000</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H12" s="28">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="10" t="s">
+      <c r="I12" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="16">
+        <v>2</v>
+      </c>
+      <c r="B13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="C13" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="17">
-        <v>155000</v>
-      </c>
-      <c r="H9" s="37">
+      <c r="E13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="18">
+        <v>12750</v>
+      </c>
+      <c r="H13" s="28">
         <f t="shared" si="0"/>
-        <v>1550</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="17">
-        <v>155000</v>
-      </c>
-      <c r="H10" s="37">
-        <f t="shared" si="0"/>
-        <v>1550</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="29">
-        <v>3</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="32">
-        <v>50000</v>
-      </c>
-      <c r="H11" s="57">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
-        <v>3</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="32">
-        <v>50000</v>
-      </c>
-      <c r="H12" s="57">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I12" s="33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="29">
-        <v>3</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="32">
-        <v>50000</v>
-      </c>
-      <c r="H13" s="57">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>20</v>
+        <v>127.5</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.35">
@@ -2353,20 +3739,20 @@
         <v>41</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="17">
-        <v>12750</v>
-      </c>
-      <c r="H14" s="37">
+        <v>10</v>
+      </c>
+      <c r="G14" s="12">
+        <v>50000</v>
+      </c>
+      <c r="H14" s="31">
         <f t="shared" si="0"/>
-        <v>127.5</v>
+        <v>500</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.35">
@@ -2383,50 +3769,50 @@
         <v>41</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="17">
-        <v>12750</v>
-      </c>
-      <c r="H15" s="37">
+        <v>10</v>
+      </c>
+      <c r="G15" s="12">
+        <v>50000</v>
+      </c>
+      <c r="H15" s="31">
         <f t="shared" si="0"/>
-        <v>127.5</v>
+        <v>500</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="29">
-        <v>3</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="10">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="32">
-        <v>4500</v>
-      </c>
-      <c r="H16" s="57">
+      <c r="C16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="12">
+        <v>50000</v>
+      </c>
+      <c r="H16" s="31">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>8</v>
+        <v>500</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -2443,20 +3829,20 @@
         <v>41</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="17">
-        <v>50000</v>
-      </c>
-      <c r="H17" s="37">
+        <v>18</v>
+      </c>
+      <c r="G17" s="12">
+        <v>155000</v>
+      </c>
+      <c r="H17" s="31">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>1550</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -2473,20 +3859,20 @@
         <v>41</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="17">
-        <v>50000</v>
-      </c>
-      <c r="H18" s="37">
+        <v>18</v>
+      </c>
+      <c r="G18" s="12">
+        <v>155000</v>
+      </c>
+      <c r="H18" s="31">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>1550</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
@@ -2503,98 +3889,98 @@
         <v>41</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="17">
-        <v>50000</v>
-      </c>
-      <c r="H19" s="37">
+        <v>18</v>
+      </c>
+      <c r="G19" s="12">
+        <v>155000</v>
+      </c>
+      <c r="H19" s="31">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>1550</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="19">
-        <v>2</v>
-      </c>
-      <c r="B20" s="19" t="s">
+      <c r="A20" s="10">
+        <v>1</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="20" t="s">
+      <c r="C20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="21" t="s">
+      <c r="E20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="12">
         <v>12750</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="31">
         <f t="shared" si="0"/>
         <v>127.5</v>
       </c>
-      <c r="I20" s="23" t="s">
-        <v>14</v>
+      <c r="I20" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="24">
-        <v>4</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="25" t="s">
+      <c r="A21" s="10">
+        <v>1</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="26" t="s">
+      <c r="E21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="27">
-        <v>4500</v>
-      </c>
-      <c r="H21" s="40">
+      <c r="G21" s="12">
+        <v>12750</v>
+      </c>
+      <c r="H21" s="31">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I21" s="28" t="s">
-        <v>14</v>
+        <v>127.5</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I21" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I21">
-      <sortCondition ref="I1:I21"/>
+      <sortCondition ref="C1:C21"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252231F1-1CC9-4F6C-A7C1-0482E23AA5FE}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2631,7 +4017,7 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="14" t="s">
@@ -2660,23 +4046,23 @@
       <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="12">
         <v>155000</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="31">
         <f t="shared" ref="H2:H4" si="0">G2/100</f>
         <v>1550</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
@@ -2697,21 +4083,21 @@
       <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="12">
         <v>155000</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="31">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
@@ -2732,138 +4118,138 @@
       <c r="F4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="12">
         <v>155000</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="31">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
+      <c r="A6" s="16">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="22">
+      <c r="F6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="18">
         <v>155000</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="28">
         <v>1550</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
     </row>
     <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+      <c r="A7" s="16">
         <v>2</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="22">
+      <c r="F7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="18">
         <v>155000</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="28">
         <v>1550</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="19">
+      <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="22">
+      <c r="F8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="18">
         <v>155000</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="28">
         <v>1550</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>21</v>
@@ -2871,35 +4257,36 @@
       <c r="F10" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="26">
         <v>50000</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="45">
+        <f t="shared" ref="H10:H12" si="1">G10/100</f>
         <v>500</v>
       </c>
-      <c r="I10" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
+      <c r="I10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
     </row>
     <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="26" t="s">
         <v>23</v>
@@ -2907,33 +4294,34 @@
       <c r="F11" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="26">
         <v>50000</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="45">
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="I11" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
+      <c r="I11" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
     </row>
     <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>25</v>
@@ -2941,130 +4329,217 @@
       <c r="F12" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <v>50000</v>
       </c>
-      <c r="H12" s="40">
-        <v>500</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-    </row>
-    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="29">
-        <v>3</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="32">
-        <v>50000</v>
-      </c>
-      <c r="H14" s="57">
-        <f t="shared" ref="H14:H16" si="1">G14/100</f>
-        <v>500</v>
-      </c>
-      <c r="I14" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" s="38"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-    </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="29">
-        <v>3</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="32">
-        <v>50000</v>
-      </c>
-      <c r="H15" s="57">
+      <c r="H12" s="45">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="I15" s="33" t="s">
+      <c r="I12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="68"/>
+    </row>
+    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="20">
+        <v>4</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="22">
+        <v>50000</v>
+      </c>
+      <c r="H14" s="32">
+        <v>500</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="68"/>
+    </row>
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="20">
+        <v>4</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="22">
+        <v>50000</v>
+      </c>
+      <c r="H15" s="32">
+        <v>500</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="68"/>
     </row>
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="29">
-        <v>3</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="20">
+        <v>4</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="31" t="s">
+      <c r="C16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="32">
+      <c r="F16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="22">
         <v>50000</v>
       </c>
-      <c r="H16" s="57">
-        <f t="shared" si="1"/>
+      <c r="H16" s="32">
         <v>500</v>
       </c>
-      <c r="I16" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="38"/>
-      <c r="M16" s="38"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H17" s="35"/>
+      <c r="I16" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="2:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="B18" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+    </row>
+    <row r="19" spans="2:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="B19" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+    </row>
+    <row r="20" spans="2:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="B20" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+    </row>
+    <row r="21" spans="2:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="B21" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+    </row>
+    <row r="22" spans="2:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="B22" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+    </row>
+    <row r="23" spans="2:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="B23" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3077,12 +4552,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4629A2-434E-4B06-B530-854874F734D8}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3098,7 +4573,7 @@
     <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3117,7 +4592,7 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="14" t="s">
@@ -3127,7 +4602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -3146,24 +4621,18 @@
       <c r="F2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="12">
         <v>155000</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="31">
         <f t="shared" ref="H2:H4" si="0">G2/100</f>
         <v>1550</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-    </row>
-    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -3182,24 +4651,18 @@
       <c r="F3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="12">
         <v>155000</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="31">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-    </row>
-    <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -3218,283 +4681,253 @@
       <c r="F4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="12">
         <v>155000</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="31">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-    </row>
-    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="H5" s="43">
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="35">
         <f>SUM(H2:H4)</f>
         <v>4650</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-    </row>
-    <row r="6" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="16">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="22">
+      <c r="F6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="18">
         <v>155000</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="28">
         <v>1550</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-    </row>
-    <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="16">
         <v>2</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="22">
+      <c r="F7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="18">
         <v>155000</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="28">
         <v>1550</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-    </row>
-    <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="19">
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="22">
+      <c r="F8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="18">
         <v>155000</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="28">
         <v>1550</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-    </row>
-    <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H9" s="41">
+    </row>
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H9" s="33">
         <f>SUM(H5:H8)</f>
         <v>9300</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="29">
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="24">
         <v>3</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="32">
+      <c r="F10" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="26">
         <v>50000</v>
       </c>
-      <c r="H10" s="57">
+      <c r="H10" s="45">
         <f t="shared" ref="H10:H12" si="1">G10/100</f>
         <v>500</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="29">
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="24">
         <v>3</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="32">
+      <c r="F11" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="26">
         <v>50000</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="45">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="24">
         <v>3</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="32">
+      <c r="F12" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="26">
         <v>50000</v>
       </c>
-      <c r="H12" s="57">
+      <c r="H12" s="45">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="42"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="44">
+    <row r="13" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="36">
         <f>SUM(H10:H12)</f>
         <v>1500</v>
       </c>
-      <c r="I13" s="42"/>
-    </row>
-    <row r="14" spans="1:16" s="46" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="56"/>
-    </row>
-    <row r="15" spans="1:16" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="50"/>
-    </row>
-    <row r="16" spans="1:16" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C16" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="65">
+      <c r="I13" s="34"/>
+    </row>
+    <row r="14" spans="1:9" s="37" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="72"/>
+    </row>
+    <row r="15" spans="1:9" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="1:9" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C16" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="40"/>
+      <c r="E16" s="53">
         <v>4650</v>
       </c>
-      <c r="F16" s="50"/>
-    </row>
-    <row r="17" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C17" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="65">
+      <c r="F16" s="41"/>
+    </row>
+    <row r="17" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C17" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="53">
         <v>4650</v>
       </c>
-      <c r="F17" s="50"/>
+      <c r="F17" s="41"/>
       <c r="H17" s="73"/>
       <c r="I17" s="73"/>
       <c r="J17" s="73"/>
@@ -3503,16 +4936,16 @@
       <c r="M17" s="73"/>
       <c r="N17" s="73"/>
     </row>
-    <row r="18" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C18" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="61">
+    <row r="18" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C18" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="49">
         <f>SUM(E16:E17)</f>
         <v>9300</v>
       </c>
-      <c r="F18" s="58"/>
+      <c r="F18" s="46"/>
       <c r="H18" s="73"/>
       <c r="I18" s="73"/>
       <c r="J18" s="73"/>
@@ -3521,54 +4954,54 @@
       <c r="M18" s="73"/>
       <c r="N18" s="73"/>
     </row>
-    <row r="19" spans="3:14" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="C19" s="67"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="69"/>
-    </row>
-    <row r="20" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C20" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="64">
+    <row r="19" spans="3:14" s="54" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
+    </row>
+    <row r="20" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C20" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="50"/>
+      <c r="E20" s="52">
         <v>1500</v>
       </c>
-      <c r="F20" s="50"/>
-    </row>
-    <row r="21" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="50"/>
-      <c r="H21" s="47"/>
-    </row>
-    <row r="22" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C22" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="74">
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C22" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="59"/>
+      <c r="E22" s="61">
         <f>E18-E20</f>
         <v>7800</v>
       </c>
-      <c r="F22" s="72"/>
-    </row>
-    <row r="23" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="50"/>
-    </row>
-    <row r="24" spans="3:14" s="46" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="53"/>
-    </row>
-    <row r="25" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="3:14" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
+      <c r="F22" s="60"/>
+    </row>
+    <row r="23" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41"/>
+    </row>
+    <row r="24" spans="3:14" s="37" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+    </row>
+    <row r="25" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C14:F14"/>

</xml_diff>

<commit_message>
Consolidando os Saldos Finais, Vendedor e Afiliado
</commit_message>
<xml_diff>
--- a/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
+++ b/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\CANDIDATURAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\Modelo5\backend\api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B87BEE-4419-4213-A151-1F913EBA744E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7AA920-F544-4056-BB97-7D154BD808C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUISITOS DO PROJETO" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="193">
   <si>
     <t>TIPO</t>
   </si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t>4. Exibir o saldo final do produtor</t>
-  </si>
-  <si>
-    <t>5. Exibir o saldo final de um afiliado</t>
   </si>
   <si>
     <t>6. Fazer tratamento de erros no backend, e reportar mensagens de erro amigáveis</t>
@@ -782,6 +779,140 @@
       <t>A documentação pode ser em</t>
     </r>
   </si>
+  <si>
+    <t>{'CURSO DE BEM-ESTAR': {'seller': 'JOSE CARLOS', 'price': 25500}, 'DOMINANDO INVESTIMENTOS': {'seller': 'MARIA CANDIDA', 'price': 150000}, 'DESENVOLVEDOR FULL STACK': {'seller': 'ELIANA NOGUEIRA', 'price': 465000}}</t>
+  </si>
+  <si>
+    <t>{'CURSO DE BEM-ESTAR': {'seller': 'JOSE CARLOS', 'price': 38250}, 'DOMINANDO INVESTIMENTOS': {'seller': 'MARIA CANDIDA', 'price': 150000}, 'DESENVOLVEDOR FULL STACK': {'seller': 'ELIANA NOGUEIRA', 'price': 930000}}</t>
+  </si>
+  <si>
+    <t>{'CURSO DE BEM-ESTAR': {'seller': 'JOSE CARLOS', 'price': 33750}, 'DOMINANDO INVESTIMENTOS': {'seller': 'MARIA CANDIDA', 'price': 150000}, 'DESENVOLVEDOR FULL STACK': {'seller': 'ELIANA NOGUEIRA', 'price': 780000}}</t>
+  </si>
+  <si>
+    <t>{'CURSO DE BEM-ESTAR': {'affiliate': 'THIAGO OLIVEIRA', 'price': 4500}, 'DESENVOLVEDOR FULL STACK': {'affiliate': 'CARLOS BATISTA', 'price': 150000}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'THIAGO OLIVEIRA': {'affiliate': 'THIAGO OLIVEIRA', 'price': 4500}, 'CARLOS BATISTA': {'affiliate': 'CARLOS BATISTA', 'price': </t>
+  </si>
+  <si>
+    <t>50000}, 'CAROLINA MACHADO': {'affiliate': 'CAROLINA MACHADO', 'price': 50000}, 'CELSO DE MELO': {'affiliate': 'CELSO DE MELO', 'price': 50000}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'JOSE_CARLOS': {'CURSO DE BEM-ESTAR': {'person': 'JOSE_CARLOS', 'price': 21000}}, 'MARIA_CANDIDA': {'DOMINANDO INVESTIMENTOS': </t>
+  </si>
+  <si>
+    <t>{'person': 'MARIA_CANDIDA', 'price': 150000}}, 'THIAGO_OLIVEIRA': {}, 'ELIANA_NOGUEIRA': {'DESENVOLVEDOR FULL STACK': {'person': 'ELIANA_NOGUEIRA', 'price': 315000}}, 'CARLOS_BATISTA': {}, 'CAROLINA_MACHADO': {}, 'CELSO_DE_MELO': {}}</t>
+  </si>
+  <si>
+    <t>{'CURSO DE BEM-ESTAR': {'affiliate': 'THIAGO_OLIVEIRA', 'price': 4500}, 'DESENVOLVEDOR FULL STACK': {'affiliate': 'CARLOS_BATISTA', 'price': 150000}}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Exibir o saldo final </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>de um</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> afiliado</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">{'JOSE_CARLOS': {'CURSO DE BEM-ESTAR': {'person': 'JOSE_CARLOS', 'price': 25500, 'price_affiliate': 0}}, 'MARIA_CANDIDA': {'DOMINANDO INVESTIMENTOS': {'person': 'MARIA_CANDIDA', 'price': 150000, 'price_affiliate': 0}}, 'THIAGO_OLIVEIRA': {}, 'ELIANA_NOGUEIRA': {'DESENVOLVEDOR FULL STACK': {'person': 'ELIANA_NOGUEIRA', </t>
+  </si>
+  <si>
+    <t>'price': 465000, 'price_affiliate': 0}}, 'CARLOS_BATISTA': {}, 'CAROLINA_MACHADO': {}, 'CELSO_DE_MELO': {}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{'total_sell_affiliate': 12750, 'total_comission_payed': 4500, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">'peson': 'JOSE_CARLOS', 'product': 'CURSO DE BEM-ESTAR'}, {'total_sell_affiliate': 0, 'total_comission_payed': 0, 'peson': 'MARIA_CANDIDA', 'product': 'DOMINANDO INVESTIMENTOS'}, {'total_sell_affiliate': 465000, 'total_comission_payed': 150000, 'peson': 'ELIANA_NOGUEIRA', 'product': 'DESENVOLVEDOR FULL STACK'}] </t>
+  </si>
+  <si>
+    <t>[{</t>
+  </si>
+  <si>
+    <t>'total_sell_affiliate': 12750,</t>
+  </si>
+  <si>
+    <t>'total_comission_payed': 4500,</t>
+  </si>
+  <si>
+    <t>'total': 38250,</t>
+  </si>
+  <si>
+    <t>'liquido': 33750,</t>
+  </si>
+  <si>
+    <t>'product': 'CURSO DE BEM-ESTAR',</t>
+  </si>
+  <si>
+    <t>'total_sell_productor': 25500,</t>
+  </si>
+  <si>
+    <t>'peson': 'JOSE_CARLOS'</t>
+  </si>
+  <si>
+    <t>}, {</t>
+  </si>
+  <si>
+    <t>'total_sell_affiliate': 0,</t>
+  </si>
+  <si>
+    <t>'total_comission_payed': 0,</t>
+  </si>
+  <si>
+    <t>'total': 150000,</t>
+  </si>
+  <si>
+    <t>'liquido': 150000,</t>
+  </si>
+  <si>
+    <t>'product': 'DOMINANDO INVESTIMENTOS',</t>
+  </si>
+  <si>
+    <t>'total_sell_productor': 150000,</t>
+  </si>
+  <si>
+    <t>'peson': 'MARIA_CANDIDA'</t>
+  </si>
+  <si>
+    <t>'total_sell_affiliate': 465000,</t>
+  </si>
+  <si>
+    <t>'total_comission_payed': 150000,</t>
+  </si>
+  <si>
+    <t>'total': 930000,</t>
+  </si>
+  <si>
+    <t>'liquido': 780000,</t>
+  </si>
+  <si>
+    <t>'product': 'DESENVOLVEDOR FULL STACK',</t>
+  </si>
+  <si>
+    <t>'total_sell_productor': 465000,</t>
+  </si>
+  <si>
+    <t>'peson': 'ELIANA_NOGUEIRA'</t>
+  </si>
+  <si>
+    <t>}]</t>
+  </si>
 </sst>
 </file>
 
@@ -790,7 +921,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,12 +957,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Ubuntu Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="16"/>
@@ -932,8 +1057,20 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Ubuntu Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -985,6 +1122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1115,10 +1258,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1201,7 +1345,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1209,104 +1352,112 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1618,10 +1769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EBEA93-B706-48A3-924F-8B7166C6FDE2}">
-  <dimension ref="A1:A140"/>
+  <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,633 +1781,641 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="64" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66"/>
+      <c r="A2" s="65"/>
     </row>
     <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="66" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
+      <c r="A4" s="65"/>
     </row>
     <row r="5" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="64" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
+      <c r="A6" s="65"/>
     </row>
     <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="66" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="66" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="66" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
+      <c r="A10" s="65"/>
     </row>
     <row r="11" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="66" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="67" t="s">
+    <row r="13" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="65"/>
+    </row>
+    <row r="15" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="66" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="67" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="66"/>
-    </row>
-    <row r="15" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
+    <row r="16" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="66" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="67" t="s">
+    <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="65"/>
+    </row>
+    <row r="19" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="66" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
-    </row>
-    <row r="19" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
+    <row r="20" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="66" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+    <row r="21" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="65"/>
+    </row>
+    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="66" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="66" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="66"/>
-    </row>
-    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="67" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="65"/>
+    </row>
+    <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="65"/>
+    </row>
+    <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="66" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="67" t="s">
+    <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="66" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="65"/>
+    </row>
+    <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="64" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="65"/>
+    </row>
+    <row r="38" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="66" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="65"/>
+    </row>
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="70"/>
+    </row>
+    <row r="41" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="70"/>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="70"/>
+    </row>
+    <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="70"/>
+    </row>
+    <row r="44" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="66" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="66" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="71"/>
+    </row>
+    <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="71"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="65"/>
+    </row>
+    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="64" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="65"/>
+    </row>
+    <row r="51" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="66" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="66" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="66" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
-    </row>
-    <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
-    </row>
-    <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="67" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="67" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="67" t="s">
+    <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="B56" s="70"/>
+    </row>
+    <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="70"/>
+    </row>
+    <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="66" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="66" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="66" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="65"/>
+    </row>
+    <row r="65" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="66" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="65"/>
+    </row>
+    <row r="69" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="65"/>
+    </row>
+    <row r="72" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="66" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="66" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="65"/>
+    </row>
+    <row r="76" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="65"/>
+    </row>
+    <row r="78" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="66" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="65"/>
+    </row>
+    <row r="80" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="69" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="64" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="69" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="67" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="65"/>
+    </row>
+    <row r="86" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="65"/>
+    </row>
+    <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="66" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="66" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="65"/>
+    </row>
+    <row r="96" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="65"/>
+    </row>
+    <row r="98" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="65"/>
+    </row>
+    <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="66" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="66" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="66" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="65"/>
+    </row>
+    <row r="107" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="64" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="65"/>
+    </row>
+    <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="66" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="65"/>
+    </row>
+    <row r="111" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="69" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="66" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="66" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="69" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="65"/>
+    </row>
+    <row r="121" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="65"/>
+    </row>
+    <row r="123" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="66" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="66" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A125" s="66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="66" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="67" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="67" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="66"/>
-    </row>
-    <row r="36" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="65" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
-    </row>
-    <row r="38" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="67" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="66"/>
-    </row>
-    <row r="40" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="67" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="67" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="67" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="67" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="67" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="67" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="66"/>
-    </row>
-    <row r="49" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="65" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="66"/>
-    </row>
-    <row r="51" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="67" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="67" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="67" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="67" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="75" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="67" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="67" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="74" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="76" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="67" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="67" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="66"/>
-    </row>
-    <row r="65" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="67" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="67" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="67" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="66"/>
-    </row>
-    <row r="69" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="67" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="67" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="66"/>
-    </row>
-    <row r="72" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="67" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="67" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="67" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="66"/>
-    </row>
-    <row r="76" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="65" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="66"/>
-    </row>
-    <row r="78" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A78" s="67" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="66"/>
-    </row>
-    <row r="80" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="76" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="65" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="67" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="76" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="74" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="66"/>
-    </row>
-    <row r="86" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="65" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="66"/>
-    </row>
-    <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A89" s="67" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A90" s="67" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A91" s="67" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A92" s="67" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A93" s="67" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A94" s="67" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="66"/>
-    </row>
-    <row r="96" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A96" s="65" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="66"/>
-    </row>
-    <row r="98" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="67" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="66"/>
-    </row>
-    <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A100" s="67" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="67" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A102" s="67" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A103" s="67" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A104" s="67" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A105" s="67" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="66"/>
-    </row>
-    <row r="107" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A107" s="65" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="66"/>
-    </row>
-    <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="67" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="66"/>
-    </row>
-    <row r="111" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="76" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="76" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A113" s="67" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A114" s="67" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A115" s="67" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A116" s="67" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A117" s="67" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A118" s="76" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A119" s="67" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="66"/>
-    </row>
-    <row r="121" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A121" s="65" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="66"/>
-    </row>
-    <row r="123" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A123" s="67" t="s">
+    <row r="127" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="66" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="66" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="65"/>
+    </row>
+    <row r="130" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="65"/>
+    </row>
+    <row r="132" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="65"/>
+    </row>
+    <row r="134" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="65"/>
+    </row>
+    <row r="138" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="66" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A124" s="67" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A125" s="67" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A126" s="67" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A127" s="67" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A128" s="67" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="66"/>
-    </row>
-    <row r="130" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A130" s="65" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="66"/>
-    </row>
-    <row r="132" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A132" s="67" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="66"/>
-    </row>
-    <row r="134" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="67" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A135" s="67" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="65"/>
+    </row>
+    <row r="140" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A140" s="64" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A136" s="67" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="66"/>
-    </row>
-    <row r="138" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A138" s="67" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="66"/>
-    </row>
-    <row r="140" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A140" s="65" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2270,7 +2429,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:Q9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,130 +2498,130 @@
     </row>
     <row r="4" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="63"/>
-      <c r="Q4" s="63"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
     </row>
     <row r="6" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="63"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="63"/>
-      <c r="Q6" s="63"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="62"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="62"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="62"/>
     </row>
     <row r="7" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="63"/>
-      <c r="L7" s="63"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="63"/>
-      <c r="Q7" s="63"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
     </row>
     <row r="8" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>18</v>
@@ -2473,26 +2632,26 @@
       <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="62" t="s">
+      <c r="G8" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="63"/>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="62"/>
     </row>
     <row r="9" spans="1:17" ht="24" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>18</v>
@@ -2501,56 +2660,56 @@
         <v>19</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="63"/>
-      <c r="L9" s="63"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
     </row>
     <row r="10" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="63"/>
+        <v>14</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
     </row>
     <row r="11" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>2</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>18</v>
@@ -2559,62 +2718,62 @@
         <v>19</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="64"/>
+        <v>24</v>
+      </c>
+      <c r="G12" s="63"/>
     </row>
     <row r="13" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="64"/>
+        <v>26</v>
+      </c>
+      <c r="G13" s="63"/>
     </row>
     <row r="14" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="64"/>
+        <v>8</v>
+      </c>
+      <c r="G14" s="63"/>
     </row>
     <row r="15" spans="1:17" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
@@ -2669,73 +2828,76 @@
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
+    <sortCondition ref="A1:A21"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -2745,7 +2907,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3313,10 +3475,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,7 +3496,7 @@
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3363,249 +3525,276 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="24">
-        <v>3</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="26">
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12">
+        <v>12750</v>
+      </c>
+      <c r="H2" s="30">
+        <f t="shared" ref="H2:H21" si="0">G2/100</f>
+        <v>127.5</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="75">
+        <f>SUM(G2:G3,G10)</f>
+        <v>38250</v>
+      </c>
+      <c r="K2" s="76">
+        <f>J2-G18</f>
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="12">
+        <v>12750</v>
+      </c>
+      <c r="H3" s="30">
+        <f t="shared" si="0"/>
+        <v>127.5</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="72"/>
+    </row>
+    <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="10">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="12">
+        <v>155000</v>
+      </c>
+      <c r="H4" s="30">
+        <f t="shared" si="0"/>
+        <v>1550</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <f>SUM(G4:G6)</f>
+        <v>465000</v>
+      </c>
+      <c r="K4" s="73">
+        <f>SUM(G2,G3,G10)</f>
+        <v>38250</v>
+      </c>
+      <c r="L4" s="73">
+        <f>K4-G18</f>
+        <v>33750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="10">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="12">
+        <v>155000</v>
+      </c>
+      <c r="H5" s="30">
+        <f t="shared" si="0"/>
+        <v>1550</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>1</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="12">
+        <v>155000</v>
+      </c>
+      <c r="H6" s="30">
+        <f t="shared" si="0"/>
+        <v>1550</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="12">
         <v>50000</v>
       </c>
-      <c r="H2" s="45">
-        <f t="shared" ref="H2:H21" si="0">G2/100</f>
-        <v>500</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="29"/>
-      <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="24">
-        <v>3</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="26">
-        <v>50000</v>
-      </c>
-      <c r="H3" s="45">
+      <c r="H7" s="30">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="I3" s="27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="24">
-        <v>3</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="26">
+      <c r="I7" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="12">
         <v>50000</v>
       </c>
-      <c r="H4" s="45">
+      <c r="H8" s="30">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="I4" s="27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="24">
-        <v>3</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="26">
-        <v>4500</v>
-      </c>
-      <c r="H5" s="45">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A6" s="20">
-        <v>4</v>
-      </c>
-      <c r="B6" s="20" t="s">
+      <c r="I8" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <f>SUM(J4,J11)</f>
+        <v>930000</v>
+      </c>
+      <c r="L8">
+        <f>K8-G19-G20-G21</f>
+        <v>780000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="C9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="22">
+      <c r="E9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="12">
         <v>50000</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H9" s="30">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="20">
-        <v>4</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="22">
-        <v>50000</v>
-      </c>
-      <c r="H7" s="32">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A8" s="20">
-        <v>4</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="22">
-        <v>50000</v>
-      </c>
-      <c r="H8" s="32">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="20">
-        <v>4</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="22">
-        <v>4500</v>
-      </c>
-      <c r="H9" s="32">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="I9" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>2</v>
       </c>
@@ -3619,23 +3808,23 @@
         <v>41</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G10" s="18">
-        <v>155000</v>
+        <v>12750</v>
       </c>
       <c r="H10" s="28">
         <f t="shared" si="0"/>
-        <v>1550</v>
+        <v>127.5</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>2</v>
       </c>
@@ -3649,7 +3838,7 @@
         <v>41</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>18</v>
@@ -3662,10 +3851,14 @@
         <v>1550</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+      <c r="J11">
+        <f>SUM(G11:G13)</f>
+        <v>465000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>2</v>
       </c>
@@ -3679,7 +3872,7 @@
         <v>41</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>18</v>
@@ -3692,10 +3885,10 @@
         <v>1550</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>2</v>
       </c>
@@ -3709,266 +3902,443 @@
         <v>41</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="G13" s="18">
-        <v>12750</v>
+        <v>155000</v>
       </c>
       <c r="H13" s="28">
         <f t="shared" si="0"/>
-        <v>127.5</v>
+        <v>1550</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="10">
-        <v>1</v>
-      </c>
-      <c r="B14" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="20">
+        <v>4</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="12">
-        <v>50000</v>
+      <c r="E14" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="22">
+        <v>4500</v>
       </c>
       <c r="H14" s="31">
         <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="10">
-        <v>1</v>
-      </c>
-      <c r="B15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="20">
+        <v>4</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="E15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="22">
         <v>50000</v>
       </c>
       <c r="H15" s="31">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="10">
-        <v>1</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="I15" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="20">
+        <v>4</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="E16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="22">
         <v>50000</v>
       </c>
       <c r="H16" s="31">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="I16" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A17" s="10">
-        <v>1</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="I16" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16">
+        <f>SUM(G14:G17)</f>
+        <v>154500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="20">
+        <v>4</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="11" t="s">
+      <c r="C17" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="12">
-        <v>155000</v>
+      <c r="E17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="22">
+        <v>50000</v>
       </c>
       <c r="H17" s="31">
         <f t="shared" si="0"/>
-        <v>1550</v>
-      </c>
-      <c r="I17" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17">
+        <v>154500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="24">
+        <v>3</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="26">
+        <v>4500</v>
+      </c>
+      <c r="H18" s="44">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="24">
+        <v>3</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="26">
+        <v>50000</v>
+      </c>
+      <c r="H19" s="44">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="I19" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="12">
-        <v>155000</v>
-      </c>
-      <c r="H18" s="31">
+    <row r="20" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="24">
+        <v>3</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="26">
+        <v>50000</v>
+      </c>
+      <c r="H20" s="44">
         <f t="shared" si="0"/>
-        <v>1550</v>
-      </c>
-      <c r="I18" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="I20" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="10">
-        <v>1</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="12">
-        <v>155000</v>
-      </c>
-      <c r="H19" s="31">
+    <row r="21" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A21" s="24">
+        <v>3</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="26">
+        <v>50000</v>
+      </c>
+      <c r="H21" s="44">
         <f t="shared" si="0"/>
-        <v>1550</v>
-      </c>
-      <c r="I19" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="I21" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="10">
-        <v>1</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="12">
-        <v>12750</v>
-      </c>
-      <c r="H20" s="31">
-        <f t="shared" si="0"/>
-        <v>127.5</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="10">
-        <v>1</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="12">
-        <v>12750</v>
-      </c>
-      <c r="H21" s="31">
-        <f t="shared" si="0"/>
-        <v>127.5</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>8</v>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I21" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I21">
-      <sortCondition ref="C1:C21"/>
+      <sortCondition descending="1" ref="C1:C21"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3980,7 +4350,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4049,20 +4419,20 @@
       <c r="G2" s="12">
         <v>155000</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="30">
         <f t="shared" ref="H2:H4" si="0">G2/100</f>
         <v>1550</v>
       </c>
       <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="68" t="s">
+      <c r="K2" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
@@ -4086,18 +4456,18 @@
       <c r="G3" s="12">
         <v>155000</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="30">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
@@ -4121,18 +4491,18 @@
       <c r="G4" s="12">
         <v>155000</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
@@ -4162,13 +4532,13 @@
       <c r="I6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="68" t="s">
+      <c r="K6" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
     </row>
     <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
@@ -4198,11 +4568,11 @@
       <c r="I7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
@@ -4232,18 +4602,18 @@
       <c r="I8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24">
         <v>3</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>39</v>
@@ -4260,27 +4630,27 @@
       <c r="G10" s="26">
         <v>50000</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="44">
         <f t="shared" ref="H10:H12" si="1">G10/100</f>
         <v>500</v>
       </c>
       <c r="I10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="68" t="s">
+      <c r="K10" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="68"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
     </row>
     <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="24">
         <v>3</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>39</v>
@@ -4297,25 +4667,25 @@
       <c r="G11" s="26">
         <v>50000</v>
       </c>
-      <c r="H11" s="45">
+      <c r="H11" s="44">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="I11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
     </row>
     <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="24">
         <v>3</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>39</v>
@@ -4332,18 +4702,18 @@
       <c r="G12" s="26">
         <v>50000</v>
       </c>
-      <c r="H12" s="45">
+      <c r="H12" s="44">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="I12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
     </row>
     <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
@@ -4367,19 +4737,19 @@
       <c r="G14" s="22">
         <v>50000</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="31">
         <v>500</v>
       </c>
       <c r="I14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="68" t="s">
+      <c r="K14" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="68"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
     </row>
     <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="20">
@@ -4403,17 +4773,17 @@
       <c r="G15" s="22">
         <v>50000</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="31">
         <v>500</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="68"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
     </row>
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
@@ -4437,104 +4807,104 @@
       <c r="G16" s="22">
         <v>50000</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="31">
         <v>500</v>
       </c>
       <c r="I16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
-      <c r="O16" s="68"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H17" s="29"/>
     </row>
     <row r="18" spans="2:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="63"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
     </row>
     <row r="19" spans="2:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
-      <c r="I19" s="63"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="63"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
     </row>
     <row r="20" spans="2:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="63"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="62"/>
+      <c r="K20" s="62"/>
     </row>
     <row r="21" spans="2:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="63"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
+      <c r="K21" s="62"/>
     </row>
     <row r="22" spans="2:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="63"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="62"/>
+      <c r="K22" s="62"/>
     </row>
     <row r="23" spans="2:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="63"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
@@ -4554,10 +4924,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4629A2-434E-4B06-B530-854874F734D8}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4573,7 +4943,7 @@
     <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4602,7 +4972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -4624,7 +4994,7 @@
       <c r="G2" s="12">
         <v>155000</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="30">
         <f t="shared" ref="H2:H4" si="0">G2/100</f>
         <v>1550</v>
       </c>
@@ -4632,7 +5002,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -4654,7 +5024,7 @@
       <c r="G3" s="12">
         <v>155000</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="30">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
@@ -4662,7 +5032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>1</v>
       </c>
@@ -4684,7 +5054,7 @@
       <c r="G4" s="12">
         <v>155000</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="30">
         <f t="shared" si="0"/>
         <v>1550</v>
       </c>
@@ -4692,13 +5062,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="H5" s="35">
+    <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="34">
         <f>SUM(H2:H4)</f>
         <v>4650</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>2</v>
       </c>
@@ -4727,7 +5097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>2</v>
       </c>
@@ -4756,7 +5126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>2</v>
       </c>
@@ -4785,13 +5155,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="H9" s="33">
+    <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="H9" s="32">
         <f>SUM(H5:H8)</f>
         <v>9300</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="24">
         <v>3</v>
       </c>
@@ -4813,7 +5183,7 @@
       <c r="G10" s="26">
         <v>50000</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="44">
         <f t="shared" ref="H10:H12" si="1">G10/100</f>
         <v>500</v>
       </c>
@@ -4821,7 +5191,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="24">
         <v>3</v>
       </c>
@@ -4843,7 +5213,7 @@
       <c r="G11" s="26">
         <v>50000</v>
       </c>
-      <c r="H11" s="45">
+      <c r="H11" s="44">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
@@ -4851,7 +5221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="24">
         <v>3</v>
       </c>
@@ -4873,7 +5243,7 @@
       <c r="G12" s="26">
         <v>50000</v>
       </c>
-      <c r="H12" s="45">
+      <c r="H12" s="44">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
@@ -4881,127 +5251,176 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="36">
+    <row r="13" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="35">
         <f>SUM(H10:H12)</f>
         <v>1500</v>
       </c>
-      <c r="I13" s="34"/>
-    </row>
-    <row r="14" spans="1:9" s="37" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="70" t="s">
+      <c r="I13" s="33"/>
+    </row>
+    <row r="14" spans="1:16" s="36" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="72"/>
-    </row>
-    <row r="15" spans="1:9" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
-    </row>
-    <row r="16" spans="1:9" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C16" s="39" t="s">
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
+      <c r="H14" t="s">
+        <v>155</v>
+      </c>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14" s="15"/>
+      <c r="P14"/>
+    </row>
+    <row r="15" spans="1:16" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="40"/>
+      <c r="H15" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15" s="15"/>
+      <c r="P15"/>
+    </row>
+    <row r="16" spans="1:16" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C16" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="53">
+      <c r="D16" s="39"/>
+      <c r="E16" s="52">
         <v>4650</v>
       </c>
-      <c r="F16" s="41"/>
-    </row>
-    <row r="17" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C17" s="39" t="s">
+      <c r="F16" s="40"/>
+      <c r="H16" t="s">
+        <v>157</v>
+      </c>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16" s="15"/>
+      <c r="P16"/>
+    </row>
+    <row r="17" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C17" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="53">
+      <c r="D17" s="39"/>
+      <c r="E17" s="52">
         <v>4650</v>
       </c>
-      <c r="F17" s="41"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="73"/>
-      <c r="K17" s="73"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73"/>
-    </row>
-    <row r="18" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C18" s="47" t="s">
+      <c r="F17" s="74"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+    </row>
+    <row r="18" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C18" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="49">
+      <c r="D18" s="47"/>
+      <c r="E18" s="48">
         <f>SUM(E16:E17)</f>
         <v>9300</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="73"/>
-    </row>
-    <row r="19" spans="3:14" s="54" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="C19" s="55"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="57"/>
-    </row>
-    <row r="20" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C20" s="51" t="s">
+      <c r="F18" s="45"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+    </row>
+    <row r="19" spans="2:14" s="53" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C20" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="52">
+      <c r="D20" s="49"/>
+      <c r="E20" s="51">
         <v>1500</v>
       </c>
-      <c r="F20" s="41"/>
-    </row>
-    <row r="21" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="41"/>
-      <c r="H21" s="38"/>
-    </row>
-    <row r="22" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C22" s="58" t="s">
+      <c r="F20" s="74"/>
+    </row>
+    <row r="21" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C21" s="38"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C22" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="59"/>
-      <c r="E22" s="61">
+      <c r="D22" s="58"/>
+      <c r="E22" s="60">
         <f>E18-E20</f>
         <v>7800</v>
       </c>
-      <c r="F22" s="60"/>
-    </row>
-    <row r="23" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-    </row>
-    <row r="24" spans="3:14" s="37" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C24" s="42"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-    </row>
-    <row r="25" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="3:14" s="37" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
+      <c r="F22" s="59"/>
+      <c r="H22" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
+      <c r="H23" s="36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" s="36" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C14:F14"/>

</xml_diff>

<commit_message>
Add Model Report, Guardar dados Agrupados
</commit_message>
<xml_diff>
--- a/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
+++ b/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\Modelo5\backend\api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7AA920-F544-4056-BB97-7D154BD808C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F738A61-F9CE-483E-B930-7AF1A2E64177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUISITOS DO PROJETO" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="194">
   <si>
     <t>TIPO</t>
   </si>
@@ -912,6 +912,9 @@
   </si>
   <si>
     <t>}]</t>
+  </si>
+  <si>
+    <t>[{"total_sell_affiliate": 12750, "total_comission_payed": 4500, "total": 38250, "liquido": 33750, "product": "CURSO DE BEM-ESTAR", "total_sell_productor": 25500, "peson": "JOSE_CARLOS"}, {"total_sell_affiliate": 465000, "total_comission_payed": 150000, "total": 620000, "liquido": 470000, "product": "DESENVOLVEDOR FULL STACK", "total_sell_productor": 155000, "peson": "JOSE_CARLOS"}, {"total_sell_affiliate": 0, "total_comission_payed": 0, "total": 150000, "liquido": 150000, "product": "DOMINANDO INVESTIMENTOS", "total_sell_productor": 150000, "peson": "MARIA_CANDIDA"}, {"total_sell_affiliate": 465000, "total_comission_payed": 150000, "total": 930000, "liquido": 780000, "product": "DESENVOLVEDOR FULL STACK", "total_sell_productor": 465000, "peson": "ELIANA_NOGUEIRA"}]</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1454,6 +1457,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1771,7 +1775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EBEA93-B706-48A3-924F-8B7166C6FDE2}">
   <dimension ref="A1:B140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -3477,8 +3481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4190,52 +4194,55 @@
         <v>160</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>174</v>
       </c>
@@ -4924,10 +4931,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4629A2-434E-4B06-B530-854874F734D8}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:H23"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5421,6 +5428,11 @@
         <v>166</v>
       </c>
     </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="83" t="s">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C14:F14"/>

</xml_diff>

<commit_message>
Exibindo Balanço final dos Produtores
</commit_message>
<xml_diff>
--- a/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
+++ b/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\Modelo5\backend\api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F738A61-F9CE-483E-B930-7AF1A2E64177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5077B6B-079D-41F0-937B-10A55109CFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUISITOS DO PROJETO" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="196">
   <si>
     <t>TIPO</t>
   </si>
@@ -915,6 +915,12 @@
   </si>
   <si>
     <t>[{"total_sell_affiliate": 12750, "total_comission_payed": 4500, "total": 38250, "liquido": 33750, "product": "CURSO DE BEM-ESTAR", "total_sell_productor": 25500, "peson": "JOSE_CARLOS"}, {"total_sell_affiliate": 465000, "total_comission_payed": 150000, "total": 620000, "liquido": 470000, "product": "DESENVOLVEDOR FULL STACK", "total_sell_productor": 155000, "peson": "JOSE_CARLOS"}, {"total_sell_affiliate": 0, "total_comission_payed": 0, "total": 150000, "liquido": 150000, "product": "DOMINANDO INVESTIMENTOS", "total_sell_productor": 150000, "peson": "MARIA_CANDIDA"}, {"total_sell_affiliate": 465000, "total_comission_payed": 150000, "total": 930000, "liquido": 780000, "product": "DESENVOLVEDOR FULL STACK", "total_sell_productor": 465000, "peson": "ELIANA_NOGUEIRA"}]</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>[{"person": "JOSE_CARLOS", "product": "CURSO DE BEM-ESTAR", "total_sold_by_producer": 25500, "total_sold_by_affiliate": 12750, "total_commission_paid": 4500, "gross_total": 38250, "liquid": 33750}, {"person": "MARIA_CANDIDA", "product": "DOMINANDO INVESTIMENTOS", "total_sold_by_producer": 150000, "total_sold_by_affiliate": 0, "total_commission_paid": 0, "gross_total": 150000, "liquid": 150000}, {"person": "ELIANA_NOGUEIRA", "product": "DESENVOLVEDOR FULL STACK", "total_sold_by_producer": 465000, "total_sold_by_affiliate": 465000, "total_commission_paid": 150000, "gross_total": 930000, "liquid": 780000}]</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1457,7 +1463,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1773,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EBEA93-B706-48A3-924F-8B7166C6FDE2}">
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,82 +1931,87 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="66" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="66" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="65"/>
     </row>
-    <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A36" s="64" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="65"/>
     </row>
-    <row r="38" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="66" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="65"/>
     </row>
-    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A40" s="66" t="s">
         <v>76</v>
       </c>
       <c r="B40" s="70"/>
     </row>
-    <row r="41" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A41" s="66" t="s">
         <v>77</v>
       </c>
       <c r="B41" s="70"/>
     </row>
-    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A42" s="66" t="s">
         <v>78</v>
       </c>
       <c r="B42" s="70"/>
     </row>
-    <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A43" s="66" t="s">
         <v>79</v>
       </c>
       <c r="B43" s="70"/>
     </row>
-    <row r="44" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="66" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="70"/>
+    </row>
+    <row r="45" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="66" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B45" s="70"/>
+    </row>
+    <row r="46" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A46" s="66" t="s">
         <v>81</v>
       </c>
       <c r="B46" s="71"/>
     </row>
-    <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="66" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="71"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="65"/>
     </row>
     <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
@@ -3481,7 +3491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
@@ -4931,10 +4941,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4629A2-434E-4B06-B530-854874F734D8}">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5429,8 +5439,13 @@
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="83" t="s">
+      <c r="B31" t="s">
         <v>193</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando dados dos Afiliados no Relatório
</commit_message>
<xml_diff>
--- a/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
+++ b/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\Modelo5\backend\api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5077B6B-079D-41F0-937B-10A55109CFE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE24BD95-010B-4CC9-9AE6-6469601E8A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUISITOS DO PROJETO" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="197">
   <si>
     <t>TIPO</t>
   </si>
@@ -921,6 +921,9 @@
   </si>
   <si>
     <t>[{"person": "JOSE_CARLOS", "product": "CURSO DE BEM-ESTAR", "total_sold_by_producer": 25500, "total_sold_by_affiliate": 12750, "total_commission_paid": 4500, "gross_total": 38250, "liquid": 33750}, {"person": "MARIA_CANDIDA", "product": "DOMINANDO INVESTIMENTOS", "total_sold_by_producer": 150000, "total_sold_by_affiliate": 0, "total_commission_paid": 0, "gross_total": 150000, "liquid": 150000}, {"person": "ELIANA_NOGUEIRA", "product": "DESENVOLVEDOR FULL STACK", "total_sold_by_producer": 465000, "total_sold_by_affiliate": 465000, "total_commission_paid": 150000, "gross_total": 930000, "liquid": 780000}]</t>
+  </si>
+  <si>
+    <t>[{"person": "JOSE_CARLOS", "product": "CURSO_DE_BEM_ESTAR", "total_sold_by_producer": 25500, "total_sold_by_affiliate": 12750, "total_commission_paid": 4500, "gross_total": 38250, "liquid": 33750, "affiliates": {"THIAGO_OLIVEIRA": 4500}}, {"person": "MARIA_CANDIDA", "product": "DOMINANDO_INVESTIMENTOS", "total_sold_by_producer": 150000, "total_sold_by_affiliate": 0, "total_commission_paid": 0, "gross_total": 150000, "liquid": 150000, "affiliates": null}, {"person": "ELIANA_NOGUEIRA", "product": "DESENVOLVEDOR_FULL_STACK", "total_sold_by_producer": 465000, "total_sold_by_affiliate": 465000, "total_commission_paid": 150000, "gross_total": 930000, "liquid": 780000, "affiliates": {"CARLOS_BATISTA": 50000, "CAROLINA_MACHADO": 50000, "CELSO_DE_MELO": 50000}}]</t>
   </si>
 </sst>
 </file>
@@ -2442,8 +2445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7EDDACD-BA6F-4CED-8353-4C1EA0202EBE}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2921,7 +2924,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3491,8 +3494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4232,6 +4235,9 @@
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>170</v>
+      </c>
+      <c r="E44" t="s">
+        <v>196</v>
       </c>
       <c r="G44" t="s">
         <v>193</v>
@@ -4943,7 +4949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4629A2-434E-4B06-B530-854874F734D8}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+    <sheetView topLeftCell="B14" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adicionando Validações na Extração dos dados
</commit_message>
<xml_diff>
--- a/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
+++ b/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\Modelo5\backend\api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE24BD95-010B-4CC9-9AE6-6469601E8A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A88509E-40DB-4B1A-84A2-15B3C14488C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="3" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="REQUISITOS DO PROJETO" sheetId="9" r:id="rId1"/>
@@ -1274,7 +1274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1442,7 +1442,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1783,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EBEA93-B706-48A3-924F-8B7166C6FDE2}">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B45"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,13 +2005,13 @@
       <c r="A46" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="71"/>
+      <c r="B46" s="70"/>
     </row>
     <row r="47" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A47" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="71"/>
+      <c r="B47" s="70"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="65"/>
@@ -2095,146 +2094,149 @@
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="65"/>
     </row>
-    <row r="65" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="66" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="66" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A67" s="66" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="65"/>
     </row>
-    <row r="69" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A69" s="66" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A70" s="66" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="65"/>
     </row>
-    <row r="72" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A72" s="66" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A73" s="66" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A74" s="66" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="65"/>
     </row>
-    <row r="76" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A76" s="64" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="65"/>
     </row>
-    <row r="78" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A78" s="66" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="65"/>
     </row>
-    <row r="80" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A80" s="69" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B80" s="70"/>
+    </row>
+    <row r="81" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A81" s="64" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A82" s="66" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A83" s="69" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B83" s="70"/>
+    </row>
+    <row r="84" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A84" s="67" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" s="70"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="65"/>
     </row>
-    <row r="86" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A86" s="64" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="65"/>
     </row>
-    <row r="88" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="66" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A89" s="66" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A90" s="66" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A91" s="66" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A92" s="66" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A93" s="66" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A94" s="66" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="65"/>
     </row>
-    <row r="96" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A96" s="64" t="s">
         <v>116</v>
       </c>
@@ -2446,7 +2448,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E21"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3494,7 +3496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519E2629-2459-4F23-98CA-336558F71BF6}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -3571,11 +3573,11 @@
       <c r="I2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="75">
+      <c r="J2" s="74">
         <f>SUM(G2:G3,G10)</f>
         <v>38250</v>
       </c>
-      <c r="K2" s="76">
+      <c r="K2" s="75">
         <f>J2-G18</f>
         <v>33750</v>
       </c>
@@ -3609,7 +3611,7 @@
       <c r="I3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="72"/>
+      <c r="J3" s="71"/>
     </row>
     <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
@@ -3644,11 +3646,11 @@
         <f>SUM(G4:G6)</f>
         <v>465000</v>
       </c>
-      <c r="K4" s="73">
+      <c r="K4" s="72">
         <f>SUM(G2,G3,G10)</f>
         <v>38250</v>
       </c>
-      <c r="L4" s="73">
+      <c r="L4" s="72">
         <f>K4-G18</f>
         <v>33750</v>
       </c>
@@ -4449,13 +4451,13 @@
       <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="77" t="s">
+      <c r="K2" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
@@ -4486,11 +4488,11 @@
       <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
@@ -4521,11 +4523,11 @@
       <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77"/>
+      <c r="O4" s="77"/>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
@@ -4555,13 +4557,13 @@
       <c r="I6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="77" t="s">
+      <c r="K6" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="76"/>
+      <c r="O6" s="76"/>
     </row>
     <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
@@ -4591,11 +4593,11 @@
       <c r="I7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
@@ -4625,11 +4627,11 @@
       <c r="I8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="77"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24">
@@ -4660,13 +4662,13 @@
       <c r="I10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="77" t="s">
+      <c r="K10" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
     </row>
     <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="24">
@@ -4697,11 +4699,11 @@
       <c r="I11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="77"/>
-      <c r="N11" s="77"/>
-      <c r="O11" s="77"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="76"/>
     </row>
     <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="24">
@@ -4732,11 +4734,11 @@
       <c r="I12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="77"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="76"/>
+      <c r="O12" s="76"/>
     </row>
     <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
@@ -4766,13 +4768,13 @@
       <c r="I14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="77" t="s">
+      <c r="K14" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="77"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="76"/>
+      <c r="N14" s="76"/>
+      <c r="O14" s="76"/>
     </row>
     <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="20">
@@ -4802,11 +4804,11 @@
       <c r="I15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="77"/>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
+      <c r="K15" s="76"/>
+      <c r="L15" s="76"/>
+      <c r="M15" s="76"/>
+      <c r="N15" s="76"/>
+      <c r="O15" s="76"/>
     </row>
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
@@ -4836,11 +4838,11 @@
       <c r="I16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="77"/>
-      <c r="L16" s="77"/>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="77"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="76"/>
+      <c r="M16" s="76"/>
+      <c r="N16" s="76"/>
+      <c r="O16" s="76"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H17" s="29"/>
@@ -5289,12 +5291,12 @@
       <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="36" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="81"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="80"/>
       <c r="H14" t="s">
         <v>155</v>
       </c>
@@ -5353,14 +5355,14 @@
       <c r="E17" s="52">
         <v>4650</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="82"/>
-      <c r="J17" s="82"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="82"/>
-      <c r="M17" s="82"/>
-      <c r="N17" s="82"/>
+      <c r="F17" s="73"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="81"/>
+      <c r="J17" s="81"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
     </row>
     <row r="18" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C18" s="46" t="s">
@@ -5372,13 +5374,13 @@
         <v>9300</v>
       </c>
       <c r="F18" s="45"/>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="82"/>
-      <c r="M18" s="82"/>
-      <c r="N18" s="82"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="81"/>
+      <c r="J18" s="81"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
     </row>
     <row r="19" spans="2:14" s="53" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="C19" s="54"/>
@@ -5394,7 +5396,7 @@
       <c r="E20" s="51">
         <v>1500</v>
       </c>
-      <c r="F20" s="74"/>
+      <c r="F20" s="73"/>
     </row>
     <row r="21" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C21" s="38"/>

</xml_diff>

<commit_message>
Ajustes No Front, Login e Register
</commit_message>
<xml_diff>
--- a/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
+++ b/backend/api/docs/ANALISE MODELO TRANSAÇÃO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Documentos\GitHub\Modelo5\backend\api\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A88509E-40DB-4B1A-84A2-15B3C14488C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DA5AB3-0570-4F15-90EA-5388FB8DF1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA22023-2B77-4AB7-B940-23F48F0A5C6C}"/>
   </bookViews>
@@ -1274,7 +1274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1447,6 +1447,7 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1782,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86EBEA93-B706-48A3-924F-8B7166C6FDE2}">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,16 +2029,19 @@
       <c r="A51" s="66" t="s">
         <v>84</v>
       </c>
+      <c r="B51" s="70"/>
     </row>
     <row r="52" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A52" s="66" t="s">
         <v>85</v>
       </c>
+      <c r="B52" s="70"/>
     </row>
     <row r="53" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="66" t="s">
         <v>151</v>
       </c>
+      <c r="B53" s="70"/>
     </row>
     <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="66" t="s">
@@ -2065,6 +2069,7 @@
       <c r="A58" s="66" t="s">
         <v>153</v>
       </c>
+      <c r="B58" s="76"/>
     </row>
     <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A59" s="66" t="s">
@@ -2075,11 +2080,13 @@
       <c r="A60" s="67" t="s">
         <v>154</v>
       </c>
+      <c r="B60" s="70"/>
     </row>
     <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="69" t="s">
         <v>90</v>
       </c>
+      <c r="B61" s="70"/>
     </row>
     <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="66" t="s">
@@ -4451,13 +4458,13 @@
       <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="76" t="s">
+      <c r="K2" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
@@ -4488,11 +4495,11 @@
       <c r="I3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
     </row>
     <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
@@ -4523,11 +4530,11 @@
       <c r="I4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
@@ -4557,13 +4564,13 @@
       <c r="I6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="76" t="s">
+      <c r="K6" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
+      <c r="L6" s="77"/>
+      <c r="M6" s="77"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
     </row>
     <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
@@ -4593,11 +4600,11 @@
       <c r="I7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
@@ -4627,11 +4634,11 @@
       <c r="I8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="77"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="24">
@@ -4662,13 +4669,13 @@
       <c r="I10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="76" t="s">
+      <c r="K10" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="77"/>
     </row>
     <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="24">
@@ -4699,11 +4706,11 @@
       <c r="I11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="76"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="76"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
     </row>
     <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="24">
@@ -4734,11 +4741,11 @@
       <c r="I12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="76"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="76"/>
-      <c r="N12" s="76"/>
-      <c r="O12" s="76"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
     </row>
     <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="20">
@@ -4768,13 +4775,13 @@
       <c r="I14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="76" t="s">
+      <c r="K14" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="76"/>
-      <c r="M14" s="76"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="76"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
     </row>
     <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="20">
@@ -4804,11 +4811,11 @@
       <c r="I15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="77"/>
+      <c r="N15" s="77"/>
+      <c r="O15" s="77"/>
     </row>
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="20">
@@ -4838,11 +4845,11 @@
       <c r="I16" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H17" s="29"/>
@@ -5291,12 +5298,12 @@
       <c r="I13" s="33"/>
     </row>
     <row r="14" spans="1:16" s="36" customFormat="1" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="81"/>
       <c r="H14" t="s">
         <v>155</v>
       </c>
@@ -5356,13 +5363,13 @@
         <v>4650</v>
       </c>
       <c r="F17" s="73"/>
-      <c r="H17" s="81"/>
-      <c r="I17" s="81"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="82"/>
+      <c r="L17" s="82"/>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
     </row>
     <row r="18" spans="2:14" s="36" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C18" s="46" t="s">
@@ -5374,13 +5381,13 @@
         <v>9300</v>
       </c>
       <c r="F18" s="45"/>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
     </row>
     <row r="19" spans="2:14" s="53" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="C19" s="54"/>

</xml_diff>